<commit_message>
excel screenshot js added 13.03
</commit_message>
<xml_diff>
--- a/src/test/java/day09_excel_screenshot_jsExecutor/ulkeler.xlsx
+++ b/src/test/java/day09_excel_screenshot_jsExecutor/ulkeler.xlsx
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="574">
   <si>
     <t>Ülke (İngilizce)</t>
   </si>
@@ -1750,6 +1750,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2178,7 +2179,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="4" customWidth="true" width="25.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2194,7 +2195,7 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>573</v>
       </c>
     </row>
@@ -2211,8 +2212,8 @@
       <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
-        <v>1500000</v>
+      <c r="E2" t="n" s="0">
+        <v>1500000.0</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2326,8 +2327,8 @@
       <c r="D10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E10">
-        <v>250000</v>
+      <c r="E10" t="n" s="0">
+        <v>250000.0</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2399,8 +2400,8 @@
       <c r="D15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E15">
-        <v>54000</v>
+      <c r="E15" t="n" s="0">
+        <v>54000.0</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4884,47 +4885,47 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3">
+      <c r="B3" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="B5" s="0">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="B6" s="0">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="B10" s="0">
         <v>5</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="0">
         <v>2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="B11" s="0">
         <v>2</v>
       </c>
     </row>

</xml_diff>